<commit_message>
added new table for developmental characteristics with their stand. errors. also some minor changes to manuscript
</commit_message>
<xml_diff>
--- a/exports/tables.xlsx
+++ b/exports/tables.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="head_width" sheetId="1" r:id="rId1"/>
+    <sheet name="dev.char" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>st. dev.</t>
   </si>
@@ -38,6 +39,24 @@
   </si>
   <si>
     <t></t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>std.error</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Pupae</t>
+  </si>
+  <si>
+    <t>Tmin</t>
   </si>
 </sst>
 </file>
@@ -45,9 +64,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +81,35 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -71,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -108,11 +156,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -127,21 +186,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -448,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -538,4 +611,132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="16">
+        <v>929.35379999999998</v>
+      </c>
+      <c r="C2" s="17">
+        <v>49.110779999999998</v>
+      </c>
+      <c r="D2" s="17">
+        <v>11.399692</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0.36807020000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="18">
+        <v>233.68279999999999</v>
+      </c>
+      <c r="C3" s="19">
+        <v>27.030670000000001</v>
+      </c>
+      <c r="D3" s="19">
+        <v>15.436838</v>
+      </c>
+      <c r="E3" s="19">
+        <v>0.30478480000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="18">
+        <v>243.9451</v>
+      </c>
+      <c r="C4" s="19">
+        <v>45.301189999999998</v>
+      </c>
+      <c r="D4" s="19">
+        <v>15.689105</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.40978490000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2602.9964</v>
+      </c>
+      <c r="C5" s="19">
+        <v>297.46382</v>
+      </c>
+      <c r="D5" s="19">
+        <v>9.3754659999999994</v>
+      </c>
+      <c r="E5" s="19">
+        <v>0.84568220000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="20">
+        <v>1207.4305999999999</v>
+      </c>
+      <c r="C6" s="19">
+        <v>489.28820999999999</v>
+      </c>
+      <c r="D6" s="19">
+        <v>12.535199</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1.6237360999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mean developemnt time of all observed stages, in R and added to paper and excel table. also graph was created, but was not accepted as good.
</commit_message>
<xml_diff>
--- a/exports/tables.xlsx
+++ b/exports/tables.xlsx
@@ -4,21 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="head_width" sheetId="1" r:id="rId1"/>
     <sheet name="dev.char" sheetId="2" r:id="rId2"/>
+    <sheet name="mean.dev.time" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>st. dev.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Instar</t>
   </si>
@@ -38,18 +36,12 @@
     <t xml:space="preserve">max. </t>
   </si>
   <si>
-    <t></t>
-  </si>
-  <si>
     <t>Stage</t>
   </si>
   <si>
     <t>SET</t>
   </si>
   <si>
-    <t>std.error</t>
-  </si>
-  <si>
     <t>Egg</t>
   </si>
   <si>
@@ -57,6 +49,132 @@
   </si>
   <si>
     <t>Tmin</t>
+  </si>
+  <si>
+    <t>15.437 ±0.305</t>
+  </si>
+  <si>
+    <t>15.689 ±0.410</t>
+  </si>
+  <si>
+    <t>9.375 ±0.846</t>
+  </si>
+  <si>
+    <t>12.535 ±1.624</t>
+  </si>
+  <si>
+    <t>243.945 ±45.301</t>
+  </si>
+  <si>
+    <t>2602.996 ±297.464</t>
+  </si>
+  <si>
+    <t>1207.431 ±489.288</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>929.354 ±49.111</t>
+  </si>
+  <si>
+    <t>233.683 ±27.031</t>
+  </si>
+  <si>
+    <t>11.400 ±0.368</t>
+  </si>
+  <si>
+    <t>129.4082 ±2.186</t>
+  </si>
+  <si>
+    <t>76.95376 ±3.362</t>
+  </si>
+  <si>
+    <t>98.92067 ±3.430</t>
+  </si>
+  <si>
+    <t>335.9138 ±19.718</t>
+  </si>
+  <si>
+    <t>281.3333 ±32.550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDT* </t>
+  </si>
+  <si>
+    <t>stand. dev.</t>
+  </si>
+  <si>
+    <t>15°C</t>
+  </si>
+  <si>
+    <t>18°C</t>
+  </si>
+  <si>
+    <t>21°C</t>
+  </si>
+  <si>
+    <t>25°C</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 2: Mean development time of all observed stages of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S. watsoni</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> over the whole range of experimental temperature except the 28°C, where beetles did not breed successfully.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 1: Developmental characteristics of observed stages of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">S. watsoni </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(means and standard errors).</t>
+    </r>
+  </si>
+  <si>
+    <t>Table 3: Head widths (in millimeters) of all three larval instars of S. watsoni.</t>
   </si>
 </sst>
 </file>
@@ -66,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,9 +195,10 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="MS Reference Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -91,24 +210,58 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF93A1A1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,31 +290,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -171,50 +322,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -519,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,80 +705,89 @@
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B3" s="1">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="C2" s="7">
-        <v>0.27</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B4" s="7">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0.35</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="B5" s="18">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="E5" s="18">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.45100000000000001</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="E4" s="9">
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -615,128 +797,284 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="15"/>
+    <col min="1" max="1" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="B4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="16">
-        <v>929.35379999999998</v>
-      </c>
-      <c r="C2" s="17">
-        <v>49.110779999999998</v>
-      </c>
-      <c r="D2" s="17">
-        <v>11.399692</v>
-      </c>
-      <c r="E2" s="17">
-        <v>0.36807020000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="18">
-        <v>233.68279999999999</v>
-      </c>
-      <c r="C3" s="19">
-        <v>27.030670000000001</v>
-      </c>
-      <c r="D3" s="19">
-        <v>15.436838</v>
-      </c>
-      <c r="E3" s="19">
-        <v>0.30478480000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="18">
-        <v>243.9451</v>
-      </c>
-      <c r="C4" s="19">
-        <v>45.301189999999998</v>
-      </c>
-      <c r="D4" s="19">
-        <v>15.689105</v>
-      </c>
-      <c r="E4" s="19">
-        <v>0.40978490000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="18">
-        <v>2602.9964</v>
-      </c>
-      <c r="C5" s="19">
-        <v>297.46382</v>
-      </c>
-      <c r="D5" s="19">
-        <v>9.3754659999999994</v>
-      </c>
-      <c r="E5" s="19">
-        <v>0.84568220000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="20">
-        <v>1207.4305999999999</v>
-      </c>
-      <c r="C6" s="19">
-        <v>489.28820999999999</v>
-      </c>
-      <c r="D6" s="19">
-        <v>12.535199</v>
-      </c>
-      <c r="E6" s="19">
-        <v>1.6237360999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="F4" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="24">
+        <v>186.29329999999999</v>
+      </c>
+      <c r="C3" s="24">
+        <v>163.75</v>
+      </c>
+      <c r="D3" s="24">
+        <v>126.4649</v>
+      </c>
+      <c r="E3" s="23">
+        <v>428.57139999999998</v>
+      </c>
+      <c r="F3" s="23">
+        <v>360</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="24">
+        <v>138.27680000000001</v>
+      </c>
+      <c r="C4" s="24">
+        <v>71.00882</v>
+      </c>
+      <c r="D4" s="24">
+        <v>91.197919999999996</v>
+      </c>
+      <c r="E4" s="24">
+        <v>301.5</v>
+      </c>
+      <c r="F4" s="21">
+        <v>188</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="24">
+        <v>105.9472</v>
+      </c>
+      <c r="C5" s="24">
+        <v>64.91901</v>
+      </c>
+      <c r="D5" s="24">
+        <v>85.026120000000006</v>
+      </c>
+      <c r="E5" s="24">
+        <v>236.0909</v>
+      </c>
+      <c r="F5" s="21">
+        <v>210</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="26">
+        <v>57</v>
+      </c>
+      <c r="C6" s="26">
+        <v>48</v>
+      </c>
+      <c r="D6" s="26">
+        <v>92</v>
+      </c>
+      <c r="E6" s="26">
+        <v>240</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated description of tables
description of tables updated and also the alignment. just small changes
</commit_message>
<xml_diff>
--- a/exports/tables.xlsx
+++ b/exports/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="head_width" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Instar</t>
   </si>
@@ -82,24 +82,6 @@
   </si>
   <si>
     <t>11.400 ±0.368</t>
-  </si>
-  <si>
-    <t>129.4082 ±2.186</t>
-  </si>
-  <si>
-    <t>76.95376 ±3.362</t>
-  </si>
-  <si>
-    <t>98.92067 ±3.430</t>
-  </si>
-  <si>
-    <t>335.9138 ±19.718</t>
-  </si>
-  <si>
-    <t>281.3333 ±32.550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MDT* </t>
   </si>
   <si>
     <t>stand. dev.</t>
@@ -184,12 +166,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -330,62 +320,68 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -695,7 +691,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,33 +702,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="A1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>28</v>
+      <c r="E2" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -749,10 +745,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0.47899999999999998</v>
       </c>
       <c r="C4" s="2">
@@ -766,28 +762,28 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>0.58199999999999996</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>0.45100000000000001</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>0.52200000000000002</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -799,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,32 +807,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="A1" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="27" t="s">
         <v>9</v>
       </c>
     </row>
@@ -844,72 +840,64 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>26</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -921,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,146 +921,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="A1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="24">
+      <c r="A3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="23">
         <v>186.29329999999999</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>163.75</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>126.4649</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>428.57139999999998</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="24">
         <v>360</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="24">
+      <c r="A4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="23">
         <v>138.27680000000001</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>71.00882</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>91.197919999999996</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>301.5</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="24">
         <v>188</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="24">
+      <c r="A5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="23">
         <v>105.9472</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>64.91901</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>85.026120000000006</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>236.0909</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="24">
         <v>210</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="26">
+      <c r="A6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="25">
         <v>57</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="25">
         <v>48</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25">
         <v>92</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="25">
         <v>240</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="8"/>
+      <c r="F6" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
number of individuals in each group was counted and reported in table form. excuse why we had such a low numer of repetitions in last two groups was added to discussion.
</commit_message>
<xml_diff>
--- a/exports/tables.xlsx
+++ b/exports/tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="dev.char" sheetId="2" r:id="rId2"/>
     <sheet name="mean.dev.time" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Instar</t>
   </si>
@@ -39,16 +39,10 @@
     <t>Stage</t>
   </si>
   <si>
-    <t>SET</t>
-  </si>
-  <si>
     <t>Egg</t>
   </si>
   <si>
     <t>Pupae</t>
-  </si>
-  <si>
-    <t>Tmin</t>
   </si>
   <si>
     <t>15.437 ±0.305</t>
@@ -130,8 +124,20 @@
     </r>
   </si>
   <si>
+    <t>Table 3: Head widths (in millimeters) of all three larval instars of S. watsoni.</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Table 1: Developmental characteristics of observed stages of </t>
+      <t xml:space="preserve">Table 1: Developmental characteristics (sum of effective temperatures (k), lower developmental threshold (t)) of observed stages of </t>
     </r>
     <r>
       <rPr>
@@ -152,21 +158,18 @@
         <family val="1"/>
         <charset val="238"/>
       </rPr>
-      <t>(means and standard errors).</t>
+      <t>(means, standard errors and number of individuals).</t>
     </r>
-  </si>
-  <si>
-    <t>Table 3: Head widths (in millimeters) of all three larval instars of S. watsoni.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,7 +265,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -291,15 +294,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -312,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -320,7 +314,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -343,7 +336,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,11 +345,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -369,24 +361,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -402,7 +391,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -444,7 +433,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -476,10 +465,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,7 +499,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kancelář">
@@ -687,48 +674,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="D2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -744,11 +731,11 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0.47899999999999998</v>
       </c>
       <c r="C4" s="2">
@@ -761,29 +748,29 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>0.58199999999999996</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="15">
         <v>0.45100000000000001</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="15">
         <v>0.52200000000000002</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -792,275 +779,285 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="B3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="D4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="E4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="F4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="27">
+        <v>222</v>
+      </c>
+      <c r="C5" s="27">
+        <v>173</v>
+      </c>
+      <c r="D5" s="27">
+        <v>208</v>
+      </c>
+      <c r="E5" s="27">
+        <v>29</v>
+      </c>
+      <c r="F5" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="21">
+        <v>186.29329999999999</v>
+      </c>
+      <c r="C3" s="21">
+        <v>163.75</v>
+      </c>
+      <c r="D3" s="21">
+        <v>126.4649</v>
+      </c>
+      <c r="E3" s="22">
+        <v>428.57139999999998</v>
+      </c>
+      <c r="F3" s="22">
+        <v>360</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="21">
+        <v>138.27680000000001</v>
+      </c>
+      <c r="C4" s="21">
+        <v>71.00882</v>
+      </c>
+      <c r="D4" s="21">
+        <v>91.197919999999996</v>
+      </c>
+      <c r="E4" s="21">
+        <v>301.5</v>
+      </c>
+      <c r="F4" s="22">
+        <v>188</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="23">
-        <v>186.29329999999999</v>
-      </c>
-      <c r="C3" s="23">
-        <v>163.75</v>
-      </c>
-      <c r="D3" s="23">
-        <v>126.4649</v>
-      </c>
-      <c r="E3" s="24">
-        <v>428.57139999999998</v>
-      </c>
-      <c r="F3" s="24">
-        <v>360</v>
-      </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="B5" s="21">
+        <v>105.9472</v>
+      </c>
+      <c r="C5" s="21">
+        <v>64.91901</v>
+      </c>
+      <c r="D5" s="21">
+        <v>85.026120000000006</v>
+      </c>
+      <c r="E5" s="21">
+        <v>236.0909</v>
+      </c>
+      <c r="F5" s="22">
+        <v>210</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="23">
-        <v>138.27680000000001</v>
-      </c>
-      <c r="C4" s="23">
-        <v>71.00882</v>
-      </c>
-      <c r="D4" s="23">
-        <v>91.197919999999996</v>
-      </c>
-      <c r="E4" s="23">
-        <v>301.5</v>
-      </c>
-      <c r="F4" s="24">
-        <v>188</v>
-      </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="B6" s="23">
+        <v>57</v>
+      </c>
+      <c r="C6" s="23">
+        <v>48</v>
+      </c>
+      <c r="D6" s="23">
+        <v>92</v>
+      </c>
+      <c r="E6" s="23">
+        <v>240</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="23">
-        <v>105.9472</v>
-      </c>
-      <c r="C5" s="23">
-        <v>64.91901</v>
-      </c>
-      <c r="D5" s="23">
-        <v>85.026120000000006</v>
-      </c>
-      <c r="E5" s="23">
-        <v>236.0909</v>
-      </c>
-      <c r="F5" s="24">
-        <v>210</v>
-      </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="25">
-        <v>57</v>
-      </c>
-      <c r="C6" s="25">
-        <v>48</v>
-      </c>
-      <c r="D6" s="25">
-        <v>92</v>
-      </c>
-      <c r="E6" s="25">
-        <v>240</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="16"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="16"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new table for parameters estimates created
</commit_message>
<xml_diff>
--- a/exports/tables.xlsx
+++ b/exports/tables.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="head_width" sheetId="1" r:id="rId1"/>
     <sheet name="dev.char" sheetId="2" r:id="rId2"/>
     <sheet name="mean.dev.time" sheetId="3" r:id="rId3"/>
+    <sheet name="dev.char.model" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Instar</t>
   </si>
@@ -161,6 +162,33 @@
       <t>(means, standard errors and number of individuals).</t>
     </r>
   </si>
+  <si>
+    <t>Table 1: Summary of development constants for S. watsoni for five developmental stages  (sum of effective temperatures (k) and lower developmental threshold (t))  (means and standard errors).</t>
+  </si>
+  <si>
+    <t>Temperature range</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Df</t>
+  </si>
+  <si>
+    <t>p value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k </t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>15-25</t>
+  </si>
+  <si>
+    <t>15-21</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +284,18 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,6 +411,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,7 +752,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -782,7 +856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1062,4 +1138,176 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="D3" s="32">
+        <v>220</v>
+      </c>
+      <c r="E3" s="33">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0.9375</v>
+      </c>
+      <c r="D4" s="32">
+        <v>171</v>
+      </c>
+      <c r="E4" s="33">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="D5" s="32">
+        <v>206</v>
+      </c>
+      <c r="E5" s="33">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="34">
+        <v>0.81989999999999996</v>
+      </c>
+      <c r="D6" s="32">
+        <v>27</v>
+      </c>
+      <c r="E6" s="33">
+        <v>1.4860000000000001E-11</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="36">
+        <v>0.85629999999999995</v>
+      </c>
+      <c r="D7" s="37">
+        <v>10</v>
+      </c>
+      <c r="E7" s="38">
+        <v>1.607E-5</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some correctures to the code
typos and others...
</commit_message>
<xml_diff>
--- a/exports/tables.xlsx
+++ b/exports/tables.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="head_width" sheetId="1" r:id="rId1"/>
     <sheet name="dev.char" sheetId="2" r:id="rId2"/>
     <sheet name="mean.dev.time" sheetId="3" r:id="rId3"/>
     <sheet name="dev.char.model" sheetId="4" r:id="rId4"/>
+    <sheet name="List1" sheetId="5" r:id="rId5"/>
+    <sheet name="dev.char.model (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="49">
   <si>
     <t>Instar</t>
   </si>
@@ -189,6 +191,57 @@
   <si>
     <t>15-21</t>
   </si>
+  <si>
+    <t>Stádium</t>
+  </si>
+  <si>
+    <t>Rozsah teplot</t>
+  </si>
+  <si>
+    <t>p hodnota</t>
+  </si>
+  <si>
+    <t>Tmin (°C)</t>
+  </si>
+  <si>
+    <t>K (HD)</t>
+  </si>
+  <si>
+    <t>vajíčko</t>
+  </si>
+  <si>
+    <t>Kukla</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tabulka 1: Souhrn vývojových konstatn pro </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">S. watsoni </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(suma efektivních teplot (K)  a spodní vývojový práh (Tmin))  (průměry a standardní chyby).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -197,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +349,16 @@
       <family val="3"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -346,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,6 +509,12 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -763,9 +832,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="19" t="s">
-        <v>27</v>
-      </c>
+      <c r="A1" s="41"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -846,9 +913,14 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -982,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F6"/>
     </sheetView>
   </sheetViews>
@@ -1144,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1310,4 +1382,191 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" thickBot="1">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="D3" s="32">
+        <v>220</v>
+      </c>
+      <c r="E3" s="33">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0.9375</v>
+      </c>
+      <c r="D4" s="32">
+        <v>171</v>
+      </c>
+      <c r="E4" s="33">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="D5" s="32">
+        <v>206</v>
+      </c>
+      <c r="E5" s="33">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="34">
+        <v>0.81989999999999996</v>
+      </c>
+      <c r="D6" s="32">
+        <v>27</v>
+      </c>
+      <c r="E6" s="33">
+        <v>1.4860000000000001E-11</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="36">
+        <v>0.85629999999999995</v>
+      </c>
+      <c r="D7" s="37">
+        <v>10</v>
+      </c>
+      <c r="E7" s="38">
+        <v>1.607E-5</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="150.75" thickBot="1">
+      <c r="B12" s="40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>